<commit_message>
TL S10035, correct S10037
</commit_message>
<xml_diff>
--- a/tl/S10037.MES.BIN.xlsx
+++ b/tl/S10037.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693A6EB5-E5EE-400B-98B9-0E75A5E654A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF63610-D38C-4E04-B6EC-444CD76C2845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="6240" windowWidth="55245" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="3510" windowWidth="55245" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S10037.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
     <t>61</t>
   </si>
   <si>
-    <t>she's nods…</t>
+    <t>she nods…</t>
   </si>
   <si>
     <t>63</t>

</xml_diff>